<commit_message>
Completely working with excel and multiplier
</commit_message>
<xml_diff>
--- a/keys.xlsx
+++ b/keys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faizk\projects\trader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEBEBAE5-47AD-476A-B9F5-4DE7AD1D1852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E5F31D-6FF8-46A6-AD98-4BDA7DE59300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4180A09E-C711-47D1-B0C1-D799AC309A12}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>account_type</t>
   </si>
@@ -63,13 +63,16 @@
   </si>
   <si>
     <t>a419d2e47093d1ec60368fb30acb0ea6</t>
+  </si>
+  <si>
+    <t>multiplier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +93,16 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +121,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -164,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -176,6 +193,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA41FCA8-96B7-424A-A4B8-93518B013F4C}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,10 +540,10 @@
     <col min="1" max="1" width="15.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" style="7" customWidth="1"/>
     <col min="3" max="3" width="36" style="7" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -534,9 +553,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
+      <c r="D1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -546,8 +568,11 @@
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -556,6 +581,9 @@
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>